<commit_message>
fix: Resolve order tracking functionality and implement DTO pattern
- Fix JSON parse error in order modification by returning complete response data
- Implement OrderTrackingDTO to improve response structure and maintainability
- Add proper JWT token handling for tracking API requests
- Fix order cancellation to properly update status and permissions
- Ensure email notifications work for all order status changes
- Maintain order history with soft delete pattern for cancelled orders

Technical changes:
- Move response mapping from controller to dedicated DTO class
- Update modify/cancel endpoints to return complete order status
- Add proper authorization headers to all tracking API calls
</commit_message>
<xml_diff>
--- a/backend/orders.xlsx
+++ b/backend/orders.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Order ID</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Postcode</t>
   </si>
   <si>
@@ -53,25 +50,28 @@
     <t>1</t>
   </si>
   <si>
-    <t>asfsa</t>
-  </si>
-  <si>
-    <t>Westermo Merlin 4708</t>
-  </si>
-  <si>
-    <t>VLAN Config: Open Trunk, VLAN Assignments: VLAN 101</t>
-  </si>
-  <si>
-    <t>asfasf</t>
-  </si>
-  <si>
-    <t>asfsadf</t>
-  </si>
-  <si>
-    <t>asfas@mail.com</t>
-  </si>
-  <si>
-    <t>32142436562</t>
+    <t>69</t>
+  </si>
+  <si>
+    <t>GW1042M</t>
+  </si>
+  <si>
+    <t>VLAN Config: Specified per port, VLAN Assignments: 69</t>
+  </si>
+  <si>
+    <t>zakariyaabdirizak@outlook.com</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>VLAN Config: Open Trunk, VLAN Assignments: 69</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -127,24 +127,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.65625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.6328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.578125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="45.91796875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.578125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.85546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.75" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="4.64453125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="9.8984375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="14.10546875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="14.85546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.85546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="15.046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.421875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="50.1640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.61328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="9.75390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.03515625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="29.6484375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="16.56640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -181,42 +180,71 @@
       <c r="K1" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="1">
-        <v>11</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s" s="0">
+      <c r="K2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="I2" s="0"/>
-      <c r="J2" t="s" s="0">
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="B3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="F3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>19</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>